<commit_message>
Nam thay doi chut xiu
Nam thay doi estimate 5.2 voi them bang cong viec chut xiu
</commit_message>
<xml_diff>
--- a/Document/estimates_wbs-v1-0-0.xlsx
+++ b/Document/estimates_wbs-v1-0-0.xlsx
@@ -983,48 +983,6 @@
     <t>5.2.2.2</t>
   </si>
   <si>
-    <t>Test form Home</t>
-  </si>
-  <si>
-    <t>Test form Login</t>
-  </si>
-  <si>
-    <t>Test form Register</t>
-  </si>
-  <si>
-    <t>Test form GroupClothes</t>
-  </si>
-  <si>
-    <t>Test form ClothDetail</t>
-  </si>
-  <si>
-    <t>Test form SearchByPrice</t>
-  </si>
-  <si>
-    <t>Test form BagDetail</t>
-  </si>
-  <si>
-    <t>Test form OrderInfomation</t>
-  </si>
-  <si>
-    <t>Test form FinishOrder</t>
-  </si>
-  <si>
-    <t>Test form Products_Management</t>
-  </si>
-  <si>
-    <t>Test form GroupProducts_Management</t>
-  </si>
-  <si>
-    <t>Test form OrderManagement</t>
-  </si>
-  <si>
-    <t>Test form Customer_Management</t>
-  </si>
-  <si>
-    <t>Test form Sales_Management</t>
-  </si>
-  <si>
     <t>5.2.2.1.1</t>
   </si>
   <si>
@@ -1110,6 +1068,48 @@
   </si>
   <si>
     <t>Test class Sales</t>
+  </si>
+  <si>
+    <t>Test page Home</t>
+  </si>
+  <si>
+    <t>Test page Login</t>
+  </si>
+  <si>
+    <t>Test page Register</t>
+  </si>
+  <si>
+    <t>Test page GroupClothes</t>
+  </si>
+  <si>
+    <t>Test page ClothDetail</t>
+  </si>
+  <si>
+    <t>Test page SearchByPrice</t>
+  </si>
+  <si>
+    <t>Test page BagDetail</t>
+  </si>
+  <si>
+    <t>Test page OrderInfomation</t>
+  </si>
+  <si>
+    <t>Test page FinishOrder</t>
+  </si>
+  <si>
+    <t>Test page Products_Management</t>
+  </si>
+  <si>
+    <t>Test page GroupProducts_Management</t>
+  </si>
+  <si>
+    <t>Test page OrderManagement</t>
+  </si>
+  <si>
+    <t>Test page Customer_Management</t>
+  </si>
+  <si>
+    <t>Test page Sales_Management</t>
   </si>
 </sst>
 </file>
@@ -1258,9 +1258,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1269,6 +1266,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1576,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H144" sqref="H144"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,37 +1597,37 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="13" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="13" t="s">
         <v>64</v>
       </c>
@@ -3781,7 +3781,7 @@
       <c r="E117" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F117" s="24">
+      <c r="F117" s="23">
         <v>6</v>
       </c>
       <c r="G117" s="4"/>
@@ -3803,7 +3803,7 @@
       <c r="E118" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F118" s="24">
+      <c r="F118" s="23">
         <v>2</v>
       </c>
       <c r="G118" s="4"/>
@@ -3825,7 +3825,7 @@
       <c r="E119" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F119" s="25">
+      <c r="F119" s="24">
         <v>0.2</v>
       </c>
       <c r="G119" s="4"/>
@@ -3847,7 +3847,7 @@
       <c r="E120" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F120" s="25">
+      <c r="F120" s="24">
         <v>0.2</v>
       </c>
       <c r="G120" s="4"/>
@@ -3869,7 +3869,7 @@
       <c r="E121" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F121" s="25">
+      <c r="F121" s="24">
         <v>0.2</v>
       </c>
       <c r="G121" s="4"/>
@@ -3891,7 +3891,7 @@
       <c r="E122" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F122" s="25">
+      <c r="F122" s="24">
         <v>0.2</v>
       </c>
       <c r="G122" s="4"/>
@@ -3913,7 +3913,7 @@
       <c r="E123" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F123" s="25">
+      <c r="F123" s="24">
         <v>0.2</v>
       </c>
       <c r="G123" s="19"/>
@@ -3935,7 +3935,7 @@
       <c r="E124" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F124" s="25">
+      <c r="F124" s="24">
         <v>0.2</v>
       </c>
       <c r="G124" s="16"/>
@@ -3957,7 +3957,7 @@
       <c r="E125" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F125" s="25">
+      <c r="F125" s="24">
         <v>0.2</v>
       </c>
       <c r="G125" s="11"/>
@@ -3980,7 +3980,7 @@
       <c r="E126" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F126" s="25">
+      <c r="F126" s="24">
         <v>0.2</v>
       </c>
       <c r="G126" s="19"/>
@@ -4003,7 +4003,7 @@
       <c r="E127" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F127" s="25">
+      <c r="F127" s="24">
         <v>0.2</v>
       </c>
       <c r="G127" s="19"/>
@@ -4026,8 +4026,8 @@
       <c r="E128" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F128" s="24">
-        <v>4</v>
+      <c r="F128" s="23">
+        <v>5</v>
       </c>
       <c r="G128" s="19"/>
       <c r="H128" s="19" t="s">
@@ -4049,8 +4049,8 @@
       <c r="E129" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F129" s="24">
-        <v>2</v>
+      <c r="F129" s="23">
+        <v>3</v>
       </c>
       <c r="G129" s="19"/>
       <c r="H129" s="19" t="s">
@@ -4061,19 +4061,19 @@
     </row>
     <row r="130" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B130" s="20" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="C130" s="17">
         <v>5</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>253</v>
+        <v>282</v>
       </c>
       <c r="E130" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F130" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F130" s="24">
+        <v>0.2</v>
       </c>
       <c r="G130" s="19"/>
       <c r="H130" s="16" t="s">
@@ -4084,19 +4084,19 @@
     </row>
     <row r="131" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B131" s="20" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="C131" s="17">
         <v>5</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>254</v>
+        <v>283</v>
       </c>
       <c r="E131" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F131" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F131" s="24">
+        <v>0.2</v>
       </c>
       <c r="G131" s="19"/>
       <c r="H131" s="16" t="s">
@@ -4107,19 +4107,19 @@
     </row>
     <row r="132" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B132" s="20" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="C132" s="17">
         <v>5</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>255</v>
+        <v>284</v>
       </c>
       <c r="E132" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F132" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F132" s="24">
+        <v>0.2</v>
       </c>
       <c r="G132" s="19"/>
       <c r="H132" s="16" t="s">
@@ -4130,19 +4130,19 @@
     </row>
     <row r="133" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B133" s="20" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C133" s="17">
         <v>5</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>256</v>
+        <v>285</v>
       </c>
       <c r="E133" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F133" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F133" s="24">
+        <v>0.2</v>
       </c>
       <c r="G133" s="19"/>
       <c r="H133" s="16" t="s">
@@ -4153,19 +4153,19 @@
     </row>
     <row r="134" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B134" s="20" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="C134" s="17">
         <v>5</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="E134" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F134" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F134" s="24">
+        <v>0.2</v>
       </c>
       <c r="G134" s="19"/>
       <c r="H134" s="16" t="s">
@@ -4176,19 +4176,19 @@
     </row>
     <row r="135" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B135" s="20" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="C135" s="17">
         <v>5</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>258</v>
+        <v>287</v>
       </c>
       <c r="E135" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F135" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F135" s="24">
+        <v>0.2</v>
       </c>
       <c r="G135" s="19"/>
       <c r="H135" s="16" t="s">
@@ -4199,19 +4199,19 @@
     </row>
     <row r="136" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B136" s="20" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="C136" s="17">
         <v>5</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>259</v>
+        <v>288</v>
       </c>
       <c r="E136" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F136" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F136" s="24">
+        <v>0.2</v>
       </c>
       <c r="G136" s="19"/>
       <c r="H136" s="16" t="s">
@@ -4222,19 +4222,19 @@
     </row>
     <row r="137" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B137" s="20" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="C137" s="17">
         <v>5</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>260</v>
+        <v>289</v>
       </c>
       <c r="E137" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F137" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F137" s="24">
+        <v>0.2</v>
       </c>
       <c r="G137" s="19"/>
       <c r="H137" s="16" t="s">
@@ -4245,19 +4245,19 @@
     </row>
     <row r="138" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B138" s="20" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="C138" s="17">
         <v>5</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>261</v>
+        <v>290</v>
       </c>
       <c r="E138" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F138" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F138" s="24">
+        <v>0.2</v>
       </c>
       <c r="G138" s="19"/>
       <c r="H138" s="16" t="s">
@@ -4268,19 +4268,19 @@
     </row>
     <row r="139" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B139" s="20" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="C139" s="17">
         <v>5</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>262</v>
+        <v>291</v>
       </c>
       <c r="E139" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F139" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F139" s="24">
+        <v>0.2</v>
       </c>
       <c r="G139" s="19"/>
       <c r="H139" s="16" t="s">
@@ -4291,19 +4291,19 @@
     </row>
     <row r="140" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B140" s="20" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="C140" s="17">
         <v>5</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>263</v>
+        <v>292</v>
       </c>
       <c r="E140" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F140" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F140" s="24">
+        <v>0.2</v>
       </c>
       <c r="G140" s="19"/>
       <c r="H140" s="16" t="s">
@@ -4314,19 +4314,19 @@
     </row>
     <row r="141" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B141" s="20" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C141" s="17">
         <v>5</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>264</v>
+        <v>293</v>
       </c>
       <c r="E141" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F141" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F141" s="24">
+        <v>0.2</v>
       </c>
       <c r="G141" s="19"/>
       <c r="H141" s="16" t="s">
@@ -4337,19 +4337,19 @@
     </row>
     <row r="142" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B142" s="20" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="C142" s="17">
         <v>5</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>265</v>
+        <v>294</v>
       </c>
       <c r="E142" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F142" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F142" s="24">
+        <v>0.2</v>
       </c>
       <c r="G142" s="19"/>
       <c r="H142" s="16" t="s">
@@ -4360,19 +4360,19 @@
     </row>
     <row r="143" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B143" s="20" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="C143" s="17">
         <v>5</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>266</v>
+        <v>295</v>
       </c>
       <c r="E143" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F143" s="25">
-        <v>0.14000000000000001</v>
+      <c r="F143" s="24">
+        <v>0.2</v>
       </c>
       <c r="G143" s="19"/>
       <c r="H143" s="16" t="s">
@@ -4389,12 +4389,12 @@
         <v>4</v>
       </c>
       <c r="D144" s="10" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="E144" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F144" s="24">
+      <c r="F144" s="23">
         <v>2</v>
       </c>
       <c r="G144" s="19"/>
@@ -4406,18 +4406,18 @@
     </row>
     <row r="145" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B145" s="20" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C145" s="17">
         <v>5</v>
       </c>
-      <c r="D145" s="23" t="s">
-        <v>289</v>
+      <c r="D145" s="22" t="s">
+        <v>275</v>
       </c>
       <c r="E145" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F145" s="25">
+      <c r="F145" s="24">
         <v>0.25</v>
       </c>
       <c r="G145" s="19"/>
@@ -4429,18 +4429,18 @@
     </row>
     <row r="146" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B146" s="20" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="C146" s="17">
         <v>5</v>
       </c>
-      <c r="D146" s="23" t="s">
-        <v>290</v>
+      <c r="D146" s="22" t="s">
+        <v>276</v>
       </c>
       <c r="E146" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F146" s="25">
+      <c r="F146" s="24">
         <v>0.25</v>
       </c>
       <c r="G146" s="19"/>
@@ -4452,18 +4452,18 @@
     </row>
     <row r="147" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B147" s="20" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C147" s="17">
         <v>5</v>
       </c>
-      <c r="D147" s="23" t="s">
-        <v>291</v>
+      <c r="D147" s="22" t="s">
+        <v>277</v>
       </c>
       <c r="E147" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F147" s="25">
+      <c r="F147" s="24">
         <v>0.25</v>
       </c>
       <c r="G147" s="19"/>
@@ -4475,18 +4475,18 @@
     </row>
     <row r="148" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B148" s="20" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="C148" s="17">
         <v>5</v>
       </c>
-      <c r="D148" s="23" t="s">
-        <v>292</v>
+      <c r="D148" s="22" t="s">
+        <v>278</v>
       </c>
       <c r="E148" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F148" s="25">
+      <c r="F148" s="24">
         <v>0.25</v>
       </c>
       <c r="G148" s="19"/>
@@ -4498,18 +4498,18 @@
     </row>
     <row r="149" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B149" s="20" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="C149" s="17">
         <v>5</v>
       </c>
-      <c r="D149" s="23" t="s">
-        <v>293</v>
+      <c r="D149" s="22" t="s">
+        <v>279</v>
       </c>
       <c r="E149" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F149" s="25">
+      <c r="F149" s="24">
         <v>0.25</v>
       </c>
       <c r="G149" s="19"/>
@@ -4521,18 +4521,18 @@
     </row>
     <row r="150" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B150" s="20" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="C150" s="17">
         <v>5</v>
       </c>
-      <c r="D150" s="23" t="s">
-        <v>294</v>
+      <c r="D150" s="22" t="s">
+        <v>280</v>
       </c>
       <c r="E150" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F150" s="25">
+      <c r="F150" s="24">
         <v>0.25</v>
       </c>
       <c r="G150" s="19"/>
@@ -4544,18 +4544,18 @@
     </row>
     <row r="151" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B151" s="20" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="C151" s="17">
         <v>5</v>
       </c>
-      <c r="D151" s="23" t="s">
-        <v>295</v>
+      <c r="D151" s="22" t="s">
+        <v>281</v>
       </c>
       <c r="E151" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F151" s="25">
+      <c r="F151" s="24">
         <v>0.25</v>
       </c>
       <c r="G151" s="19"/>

</xml_diff>

<commit_message>
Thuan update tai lieu phan 5
</commit_message>
<xml_diff>
--- a/Document/estimates_wbs-v1-0-0.xlsx
+++ b/Document/estimates_wbs-v1-0-0.xlsx
@@ -1686,11 +1686,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1998,8 +1998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G177" sqref="G177"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2019,37 +2019,37 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="37"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="37"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="13" t="s">
         <v>53</v>
       </c>
@@ -4102,10 +4102,10 @@
         <v>32</v>
       </c>
       <c r="F106" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G106" s="32">
-        <v>3.4</v>
+        <v>1.8</v>
       </c>
       <c r="H106" s="32" t="s">
         <v>57</v>
@@ -4306,10 +4306,10 @@
         <v>32</v>
       </c>
       <c r="F116" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G116" s="32">
-        <v>3.4</v>
+        <v>5.4</v>
       </c>
       <c r="H116" s="32" t="s">
         <v>57</v>
@@ -4633,10 +4633,10 @@
       <c r="E132" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F132" s="38">
+      <c r="F132" s="37">
         <v>0.6</v>
       </c>
-      <c r="G132" s="38">
+      <c r="G132" s="37">
         <v>1.1000000000000001</v>
       </c>
       <c r="H132" s="32" t="s">
@@ -4657,8 +4657,8 @@
       <c r="E133" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F133" s="38"/>
-      <c r="G133" s="38"/>
+      <c r="F133" s="37"/>
+      <c r="G133" s="37"/>
       <c r="H133" s="16" t="s">
         <v>57</v>
       </c>
@@ -4677,8 +4677,8 @@
       <c r="E134" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F134" s="38"/>
-      <c r="G134" s="38"/>
+      <c r="F134" s="37"/>
+      <c r="G134" s="37"/>
       <c r="H134" s="16" t="s">
         <v>57</v>
       </c>
@@ -4697,8 +4697,8 @@
       <c r="E135" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F135" s="38"/>
-      <c r="G135" s="38"/>
+      <c r="F135" s="37"/>
+      <c r="G135" s="37"/>
       <c r="H135" s="16" t="s">
         <v>57</v>
       </c>
@@ -4717,8 +4717,8 @@
       <c r="E136" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F136" s="38"/>
-      <c r="G136" s="38"/>
+      <c r="F136" s="37"/>
+      <c r="G136" s="37"/>
       <c r="H136" s="16" t="s">
         <v>57</v>
       </c>
@@ -4737,10 +4737,10 @@
       <c r="E137" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F137" s="38">
+      <c r="F137" s="37">
         <v>0.6</v>
       </c>
-      <c r="G137" s="38">
+      <c r="G137" s="37">
         <v>1.1000000000000001</v>
       </c>
       <c r="H137" s="32" t="s">
@@ -4761,8 +4761,8 @@
       <c r="E138" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F138" s="38"/>
-      <c r="G138" s="38"/>
+      <c r="F138" s="37"/>
+      <c r="G138" s="37"/>
       <c r="H138" s="16" t="s">
         <v>57</v>
       </c>
@@ -4781,8 +4781,8 @@
       <c r="E139" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F139" s="38"/>
-      <c r="G139" s="38"/>
+      <c r="F139" s="37"/>
+      <c r="G139" s="37"/>
       <c r="H139" s="16" t="s">
         <v>57</v>
       </c>
@@ -4801,8 +4801,8 @@
       <c r="E140" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F140" s="38"/>
-      <c r="G140" s="38"/>
+      <c r="F140" s="37"/>
+      <c r="G140" s="37"/>
       <c r="H140" s="16" t="s">
         <v>57</v>
       </c>
@@ -4821,8 +4821,8 @@
       <c r="E141" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F141" s="38"/>
-      <c r="G141" s="38"/>
+      <c r="F141" s="37"/>
+      <c r="G141" s="37"/>
       <c r="H141" s="16" t="s">
         <v>57</v>
       </c>
@@ -4841,8 +4841,8 @@
       <c r="E142" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F142" s="38"/>
-      <c r="G142" s="38"/>
+      <c r="F142" s="37"/>
+      <c r="G142" s="37"/>
       <c r="H142" s="16" t="s">
         <v>57</v>
       </c>
@@ -4861,8 +4861,8 @@
       <c r="E143" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F143" s="38"/>
-      <c r="G143" s="38"/>
+      <c r="F143" s="37"/>
+      <c r="G143" s="37"/>
       <c r="H143" s="16" t="s">
         <v>57</v>
       </c>
@@ -4881,8 +4881,8 @@
       <c r="E144" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F144" s="38"/>
-      <c r="G144" s="38"/>
+      <c r="F144" s="37"/>
+      <c r="G144" s="37"/>
       <c r="H144" s="16" t="s">
         <v>57</v>
       </c>
@@ -4901,8 +4901,8 @@
       <c r="E145" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F145" s="38"/>
-      <c r="G145" s="38"/>
+      <c r="F145" s="37"/>
+      <c r="G145" s="37"/>
       <c r="H145" s="16" t="s">
         <v>57</v>
       </c>
@@ -4921,8 +4921,8 @@
       <c r="E146" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F146" s="38"/>
-      <c r="G146" s="38"/>
+      <c r="F146" s="37"/>
+      <c r="G146" s="37"/>
       <c r="H146" s="16" t="s">
         <v>57</v>
       </c>
@@ -4941,10 +4941,10 @@
       <c r="E147" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F147" s="38">
+      <c r="F147" s="37">
         <v>0.4</v>
       </c>
-      <c r="G147" s="38">
+      <c r="G147" s="37">
         <v>0.7</v>
       </c>
       <c r="H147" s="32" t="s">
@@ -4965,8 +4965,8 @@
       <c r="E148" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F148" s="38"/>
-      <c r="G148" s="38"/>
+      <c r="F148" s="37"/>
+      <c r="G148" s="37"/>
       <c r="H148" s="16" t="s">
         <v>57</v>
       </c>
@@ -4985,8 +4985,8 @@
       <c r="E149" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F149" s="38"/>
-      <c r="G149" s="38"/>
+      <c r="F149" s="37"/>
+      <c r="G149" s="37"/>
       <c r="H149" s="16" t="s">
         <v>57</v>
       </c>
@@ -5005,8 +5005,8 @@
       <c r="E150" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F150" s="38"/>
-      <c r="G150" s="38"/>
+      <c r="F150" s="37"/>
+      <c r="G150" s="37"/>
       <c r="H150" s="16" t="s">
         <v>57</v>
       </c>
@@ -5025,8 +5025,8 @@
       <c r="E151" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F151" s="38"/>
-      <c r="G151" s="38"/>
+      <c r="F151" s="37"/>
+      <c r="G151" s="37"/>
       <c r="H151" s="16" t="s">
         <v>57</v>
       </c>
@@ -5045,8 +5045,8 @@
       <c r="E152" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F152" s="38"/>
-      <c r="G152" s="38"/>
+      <c r="F152" s="37"/>
+      <c r="G152" s="37"/>
       <c r="H152" s="16" t="s">
         <v>57</v>
       </c>
@@ -5065,8 +5065,8 @@
       <c r="E153" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F153" s="38"/>
-      <c r="G153" s="38"/>
+      <c r="F153" s="37"/>
+      <c r="G153" s="37"/>
       <c r="H153" s="16" t="s">
         <v>57</v>
       </c>
@@ -5085,10 +5085,10 @@
       <c r="E154" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F154" s="38">
+      <c r="F154" s="37">
         <v>0.6</v>
       </c>
-      <c r="G154" s="38">
+      <c r="G154" s="37">
         <v>1.1000000000000001</v>
       </c>
       <c r="H154" s="32" t="s">
@@ -5109,8 +5109,8 @@
       <c r="E155" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F155" s="38"/>
-      <c r="G155" s="38"/>
+      <c r="F155" s="37"/>
+      <c r="G155" s="37"/>
       <c r="H155" s="16" t="s">
         <v>57</v>
       </c>
@@ -5129,8 +5129,8 @@
       <c r="E156" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F156" s="38"/>
-      <c r="G156" s="38"/>
+      <c r="F156" s="37"/>
+      <c r="G156" s="37"/>
       <c r="H156" s="16" t="s">
         <v>57</v>
       </c>
@@ -5149,8 +5149,8 @@
       <c r="E157" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F157" s="38"/>
-      <c r="G157" s="38"/>
+      <c r="F157" s="37"/>
+      <c r="G157" s="37"/>
       <c r="H157" s="16" t="s">
         <v>57</v>
       </c>
@@ -5169,8 +5169,8 @@
       <c r="E158" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F158" s="38"/>
-      <c r="G158" s="38"/>
+      <c r="F158" s="37"/>
+      <c r="G158" s="37"/>
       <c r="H158" s="16" t="s">
         <v>57</v>
       </c>
@@ -5189,8 +5189,8 @@
       <c r="E159" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F159" s="38"/>
-      <c r="G159" s="38"/>
+      <c r="F159" s="37"/>
+      <c r="G159" s="37"/>
       <c r="H159" s="16" t="s">
         <v>57</v>
       </c>
@@ -5209,8 +5209,8 @@
       <c r="E160" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F160" s="38"/>
-      <c r="G160" s="38"/>
+      <c r="F160" s="37"/>
+      <c r="G160" s="37"/>
       <c r="H160" s="16" t="s">
         <v>57</v>
       </c>
@@ -5229,8 +5229,8 @@
       <c r="E161" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F161" s="38"/>
-      <c r="G161" s="38"/>
+      <c r="F161" s="37"/>
+      <c r="G161" s="37"/>
       <c r="H161" s="16" t="s">
         <v>57</v>
       </c>
@@ -5249,10 +5249,10 @@
       <c r="E162" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F162" s="38">
+      <c r="F162" s="37">
         <v>0.6</v>
       </c>
-      <c r="G162" s="38">
+      <c r="G162" s="37">
         <v>1.1000000000000001</v>
       </c>
       <c r="H162" s="32" t="s">
@@ -5273,8 +5273,8 @@
       <c r="E163" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F163" s="38"/>
-      <c r="G163" s="38"/>
+      <c r="F163" s="37"/>
+      <c r="G163" s="37"/>
       <c r="H163" s="16" t="s">
         <v>57</v>
       </c>
@@ -5293,8 +5293,8 @@
       <c r="E164" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F164" s="38"/>
-      <c r="G164" s="38"/>
+      <c r="F164" s="37"/>
+      <c r="G164" s="37"/>
       <c r="H164" s="16" t="s">
         <v>57</v>
       </c>
@@ -5313,8 +5313,8 @@
       <c r="E165" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F165" s="38"/>
-      <c r="G165" s="38"/>
+      <c r="F165" s="37"/>
+      <c r="G165" s="37"/>
       <c r="H165" s="16" t="s">
         <v>57</v>
       </c>
@@ -5333,8 +5333,8 @@
       <c r="E166" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F166" s="38"/>
-      <c r="G166" s="38"/>
+      <c r="F166" s="37"/>
+      <c r="G166" s="37"/>
       <c r="H166" s="16" t="s">
         <v>57</v>
       </c>
@@ -5353,10 +5353,10 @@
       <c r="E167" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F167" s="38">
+      <c r="F167" s="37">
         <v>0.8</v>
       </c>
-      <c r="G167" s="38">
+      <c r="G167" s="37">
         <v>1.4</v>
       </c>
       <c r="H167" s="32" t="s">
@@ -5377,8 +5377,8 @@
       <c r="E168" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F168" s="38"/>
-      <c r="G168" s="38"/>
+      <c r="F168" s="37"/>
+      <c r="G168" s="37"/>
       <c r="H168" s="16" t="s">
         <v>57</v>
       </c>
@@ -5397,8 +5397,8 @@
       <c r="E169" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F169" s="38"/>
-      <c r="G169" s="38"/>
+      <c r="F169" s="37"/>
+      <c r="G169" s="37"/>
       <c r="H169" s="16" t="s">
         <v>57</v>
       </c>
@@ -5417,8 +5417,8 @@
       <c r="E170" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F170" s="38"/>
-      <c r="G170" s="38"/>
+      <c r="F170" s="37"/>
+      <c r="G170" s="37"/>
       <c r="H170" s="16" t="s">
         <v>57</v>
       </c>
@@ -5437,8 +5437,8 @@
       <c r="E171" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F171" s="38"/>
-      <c r="G171" s="38"/>
+      <c r="F171" s="37"/>
+      <c r="G171" s="37"/>
       <c r="H171" s="16" t="s">
         <v>57</v>
       </c>
@@ -5457,8 +5457,8 @@
       <c r="E172" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F172" s="38"/>
-      <c r="G172" s="38"/>
+      <c r="F172" s="37"/>
+      <c r="G172" s="37"/>
       <c r="H172" s="16" t="s">
         <v>57</v>
       </c>
@@ -5477,8 +5477,8 @@
       <c r="E173" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F173" s="38"/>
-      <c r="G173" s="38"/>
+      <c r="F173" s="37"/>
+      <c r="G173" s="37"/>
       <c r="H173" s="16" t="s">
         <v>57</v>
       </c>
@@ -5497,8 +5497,8 @@
       <c r="E174" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F174" s="38"/>
-      <c r="G174" s="38"/>
+      <c r="F174" s="37"/>
+      <c r="G174" s="37"/>
       <c r="H174" s="16" t="s">
         <v>57</v>
       </c>
@@ -5517,10 +5517,10 @@
       <c r="E175" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="F175" s="38">
+      <c r="F175" s="37">
         <v>0.4</v>
       </c>
-      <c r="G175" s="38">
+      <c r="G175" s="37">
         <v>0.7</v>
       </c>
       <c r="H175" s="32" t="s">
@@ -5541,8 +5541,8 @@
       <c r="E176" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F176" s="38"/>
-      <c r="G176" s="38"/>
+      <c r="F176" s="37"/>
+      <c r="G176" s="37"/>
       <c r="H176" s="16" t="s">
         <v>57</v>
       </c>

</xml_diff>